<commit_message>
Updated license and added save Excel function.
</commit_message>
<xml_diff>
--- a/vignettes/Iris Data.xlsx
+++ b/vignettes/Iris Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="3">
     <font>
@@ -414,13 +414,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor rgb="FF1A1B41"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>

</xml_diff>